<commit_message>
acabe la seccion 4
</commit_message>
<xml_diff>
--- a/Estructura_e_interfaz.xlsx
+++ b/Estructura_e_interfaz.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Curso de excel" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -127,6 +127,36 @@
   <si>
     <t xml:space="preserve">F7 para revisar la ortografia y correcion de esta </t>
   </si>
+  <si>
+    <t>para cambiar la letra e con control + k</t>
+  </si>
+  <si>
+    <t>para abrir documentos es con control + a</t>
+  </si>
+  <si>
+    <t>para un nuevo libro es con control + u</t>
+  </si>
+  <si>
+    <t>para la fecha es con control + coma  + punto</t>
+  </si>
+  <si>
+    <t>para la hora es con control + shift + puntos supensivos :</t>
+  </si>
+  <si>
+    <t>para pasar de un libro a otro pulsamos conntrol + f6</t>
+  </si>
+  <si>
+    <t>para cerrar un libro es control + r</t>
+  </si>
+  <si>
+    <t>para cambiar el fomato ya sea de moneda a general o viserversa se presiona control + mayuscula + uno pero los que estan arriba</t>
+  </si>
+  <si>
+    <t>PARA TACHAR ES CONTROL + MAYUSCULA + 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECCIONAR TODO ES CONTROL + E puede aplicar a las tablas </t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +166,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +205,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -204,7 +242,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,6 +250,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -499,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="XEO1" workbookViewId="0">
+      <selection activeCell="XFD4" sqref="XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,8 +578,8 @@
   </sheetPr>
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +599,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3">
@@ -570,7 +610,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4">
@@ -581,7 +621,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
@@ -592,7 +632,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -603,7 +643,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -614,7 +654,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -709,10 +749,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +803,57 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>